<commit_message>
After Initial Solution has been done: added Operator and Local Search Operator: BestInsertPlace has been done twice with different way: Now have to make Local Search 3 and optimise Local Search1(which was trip reallocation
</commit_message>
<xml_diff>
--- a/104 distance matrix.xlsx
+++ b/104 distance matrix.xlsx
@@ -346,9 +346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>